<commit_message>
added files from laptop
</commit_message>
<xml_diff>
--- a/worlds/replays.xlsx
+++ b/worlds/replays.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Michael\Desktop\minecraftWorldViewer\worlds\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\micha\Desktop\build_battle_ai\worlds\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A23CDC5B-6098-4EDD-B632-E34E5C82981D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26A5EBEE-69C7-464F-BBD4-ACD84DFA1616}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="16185" windowWidth="29040" windowHeight="15840" xr2:uid="{6A1002F9-C391-4556-9E51-20312C48F96B}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22620" windowHeight="13500" xr2:uid="{6A1002F9-C391-4556-9E51-20312C48F96B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="52">
   <si>
     <t>/replay 2da3c03b-b1e2-414a-ad15-059659ee11e9 #00e708f3</t>
   </si>
@@ -189,6 +189,9 @@
   </si>
   <si>
     <t>robot</t>
+  </si>
+  <si>
+    <t>unkown</t>
   </si>
 </sst>
 </file>
@@ -570,15 +573,15 @@
   <dimension ref="A1:B30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="55.5546875" customWidth="1"/>
+    <col min="1" max="1" width="55.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>26</v>
       </c>
@@ -586,7 +589,22 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>0</v>
       </c>
@@ -594,7 +612,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>1</v>
       </c>
@@ -602,7 +620,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>2</v>
       </c>
@@ -610,7 +628,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>3</v>
       </c>
@@ -618,7 +636,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>4</v>
       </c>
@@ -626,7 +644,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>5</v>
       </c>
@@ -634,7 +652,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>6</v>
       </c>
@@ -642,7 +660,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>7</v>
       </c>
@@ -650,7 +668,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>8</v>
       </c>
@@ -658,7 +676,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>9</v>
       </c>
@@ -666,7 +684,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>10</v>
       </c>
@@ -674,7 +692,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>11</v>
       </c>
@@ -682,7 +700,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>12</v>
       </c>
@@ -690,7 +708,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>13</v>
       </c>
@@ -698,7 +716,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>14</v>
       </c>
@@ -706,7 +724,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>15</v>
       </c>
@@ -714,7 +732,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>16</v>
       </c>
@@ -722,7 +740,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>17</v>
       </c>
@@ -730,7 +748,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>18</v>
       </c>
@@ -738,7 +756,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>19</v>
       </c>
@@ -746,7 +764,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>20</v>
       </c>
@@ -754,7 +772,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>21</v>
       </c>
@@ -762,7 +780,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>22</v>
       </c>
@@ -770,7 +788,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>23</v>
       </c>
@@ -778,7 +796,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>24</v>
       </c>
@@ -786,7 +804,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>25</v>
       </c>

</xml_diff>